<commit_message>
[AliExpress] 알리 2.0 7차 업로드
<변경사항>
1. 링크 소싱 기능 bug 수정
2. J열(동영상), K열(배송방법), L열(배송비), V열(판매자코드) 데이터 크롤링 추가
3. 배송불가한 상품 수집 안하도록 방어코드 추가(배송지 Korea로 설정시)
</commit_message>
<xml_diff>
--- a/AliExpressShoppingCrawller/driver/sheet_reference.xlsx
+++ b/AliExpressShoppingCrawller/driver/sheet_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whdgu\Desktop\Git\Python\JingDongShoppingCrawller\driver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whdgu\Desktop\Git\Python\AliExpressShoppingCrawller\driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06DF6CD-95D2-4465-B29C-F57E3519213C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3161F7-1F9A-4394-9B95-73F403B356DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2625" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,12 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
-    <t>선택제품가격</t>
-  </si>
-  <si>
-    <t>상품제목</t>
-  </si>
-  <si>
     <t>대표이미지</t>
   </si>
   <si>
@@ -58,21 +51,6 @@
     <t>고객사_상품코드</t>
   </si>
   <si>
-    <t>국내쇼핑몰이름</t>
-  </si>
-  <si>
-    <t>국내쇼핑몰등급</t>
-  </si>
-  <si>
-    <t>국내사이트</t>
-  </si>
-  <si>
-    <t>국내제품링크</t>
-  </si>
-  <si>
-    <t>이미지이름</t>
-  </si>
-  <si>
     <t>이미지저장경로</t>
   </si>
   <si>
@@ -85,19 +63,43 @@
     <t>국내사이트태그</t>
   </si>
   <si>
-    <t>리뷰수</t>
-  </si>
-  <si>
-    <t>국내사이트가격</t>
-  </si>
-  <si>
-    <t>국내사이트배송비</t>
-  </si>
-  <si>
-    <t>타오바오검색결과주소</t>
-  </si>
-  <si>
-    <t>타오바오검색선택링크주소</t>
+    <t>검색키워드</t>
+  </si>
+  <si>
+    <t>정가</t>
+  </si>
+  <si>
+    <t>할인가</t>
+  </si>
+  <si>
+    <t>댓글수</t>
+  </si>
+  <si>
+    <t>구매수</t>
+  </si>
+  <si>
+    <t>검색메인cate</t>
+  </si>
+  <si>
+    <t>상품url</t>
+  </si>
+  <si>
+    <t>상품가격범위</t>
+  </si>
+  <si>
+    <t>상품명</t>
+  </si>
+  <si>
+    <t>동영상링크</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송방법</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송비</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -105,7 +107,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -153,15 +155,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="쉼표 [0] 2" xfId="2" xr:uid="{11B08D0E-92B1-406E-812D-058D09AE90F3}"/>
@@ -469,7 +468,7 @@
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -478,71 +477,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" t="s">
         <v>5</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[AliExpress] AliExpress crawller 2.0 8차 S/W 업데이트
 -. 심플 데이터 수집 기능 추가
 -. 안쓰는 상품수집 타입 삭제
 -. 예상배송일 / 배송방법 / 배송비 / 동영상 링크 / 판매자상품코드 데이터 추가
 -. 상품수집 속도 개선
 -. 슬라이드바 체크 성능 개선 (99% 성공률)
 -. 기타 버그 수정 및 속도 개선
</commit_message>
<xml_diff>
--- a/AliExpressShoppingCrawller/driver/sheet_reference.xlsx
+++ b/AliExpressShoppingCrawller/driver/sheet_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whdgu\Desktop\Git\Python\JingDongShoppingCrawller\driver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whdgu\Desktop\Git\Python\AliExpressShoppingCrawller\driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06DF6CD-95D2-4465-B29C-F57E3519213C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2A3BF6-6DCC-452F-A3AA-E24260A88314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-180" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
-    <t>선택제품가격</t>
-  </si>
-  <si>
-    <t>상품제목</t>
-  </si>
-  <si>
     <t>대표이미지</t>
   </si>
   <si>
@@ -55,49 +49,55 @@
     <t>상세페이지</t>
   </si>
   <si>
-    <t>고객사_상품코드</t>
-  </si>
-  <si>
-    <t>국내쇼핑몰이름</t>
-  </si>
-  <si>
-    <t>국내쇼핑몰등급</t>
-  </si>
-  <si>
-    <t>국내사이트</t>
-  </si>
-  <si>
-    <t>국내제품링크</t>
-  </si>
-  <si>
-    <t>이미지이름</t>
-  </si>
-  <si>
-    <t>이미지저장경로</t>
-  </si>
-  <si>
-    <t>네이버카테고리</t>
-  </si>
-  <si>
-    <t>국내사이트제목</t>
-  </si>
-  <si>
-    <t>국내사이트태그</t>
-  </si>
-  <si>
-    <t>리뷰수</t>
-  </si>
-  <si>
-    <t>국내사이트가격</t>
-  </si>
-  <si>
-    <t>국내사이트배송비</t>
-  </si>
-  <si>
-    <t>타오바오검색결과주소</t>
-  </si>
-  <si>
-    <t>타오바오검색선택링크주소</t>
+    <t>검색키워드</t>
+  </si>
+  <si>
+    <t>정가</t>
+  </si>
+  <si>
+    <t>할인가</t>
+  </si>
+  <si>
+    <t>댓글수</t>
+  </si>
+  <si>
+    <t>구매수</t>
+  </si>
+  <si>
+    <t>상품명</t>
+  </si>
+  <si>
+    <t>예상배송일</t>
+  </si>
+  <si>
+    <t>공란1</t>
+  </si>
+  <si>
+    <t>공란2</t>
+  </si>
+  <si>
+    <t>동영상링크</t>
+  </si>
+  <si>
+    <t>배송방법</t>
+  </si>
+  <si>
+    <t>배송비</t>
+  </si>
+  <si>
+    <t>검색메인cate</t>
+  </si>
+  <si>
+    <t>상품url</t>
+  </si>
+  <si>
+    <t>상품가격범위</t>
+  </si>
+  <si>
+    <t>원본상품명</t>
+  </si>
+  <si>
+    <t>상품코드</t>
   </si>
 </sst>
 </file>
@@ -105,7 +105,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -153,15 +153,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="쉼표 [0] 2" xfId="2" xr:uid="{11B08D0E-92B1-406E-812D-058D09AE90F3}"/>
@@ -468,81 +465,92 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" t="s">
         <v>21</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>